<commit_message>
Aggiunta della funzionalità di salvataggio dei dati validi e invalidi in un database SQLite. Modifiche ai metodi di validazione per gestire i flag di correzione e miglioramento della formattazione degli errori nei report di validazione.
</commit_message>
<xml_diff>
--- a/output/invalid/customers_invalid.xlsx
+++ b/output/invalid/customers_invalid.xlsx
@@ -448,200 +448,120 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>{'id': 'da671afa-1c1c-43b2-870e-b1321e27f076', 'name': 'Eraldo Gozzano-Valmarana', 'email': 'email_non_valida', 'birth_date': '3000-01-01', 'phone_number': '+39 3917542572', 'address': 'Stretto Elvira, 273\n34012, Basovizza (TS)', 'city': 'San Genesio Atesino', 'postal_code': 'ABCDE', 'state': 'Pistoia', 'country': 'Tajikistan', 'latitude': -87.9578655, 'longitude': -54.587759}</t>
+          <t>{"id": "da671afa-1c1c-43b2-870e-b1321e27f076", "name": "Eraldo Gozzano-Valmarana", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Stretto Elvira, 273\n34012, Basovizza (TS)", "city": "San Genesio Atesino", "postal_code": "ABCDE", "state": "Pistoia", "country": "Tajikistan", "latitude": -87.9578655, "longitude": -54.587759}</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3 validation errors for Customer
-email
-  value is not a valid email address: An email address must have an @-sign. [type=value_error, input_value='email_non_valida', input_type=str]
-birth_date
-  Value error, Data di nascita deve essere nel passato [type=value_error, input_value='3000-01-01', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/value_error
-postal_code
-  Input should be a valid integer, unable to parse string as an integer [type=int_parsing, input_value='ABCDE', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/int_parsing</t>
+          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>{'id': 'a4a2a54f-3833-4d8d-9129-90cad4f58d76', 'name': 'Rosina Visintini', 'email': 'email_non_valida', 'birth_date': '3000-01-01', 'phone_number': '+39 3917542572', 'address': 'Vicolo Magnani, 43\n98141, Giampilieri Marina (ME)', 'city': 'Caprioli', 'postal_code': 'ABCDE', 'state': 'Asti', 'country': 'Giappone', 'latitude': -79.2209, 'longitude': -9.437987}</t>
+          <t>{"id": "a4a2a54f-3833-4d8d-9129-90cad4f58d76", "name": "Rosina Visintini", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Vicolo Magnani, 43\n98141, Giampilieri Marina (ME)", "city": "Caprioli", "postal_code": "ABCDE", "state": "Asti", "country": "Giappone", "latitude": -79.2209, "longitude": -9.437987}</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3 validation errors for Customer
-email
-  value is not a valid email address: An email address must have an @-sign. [type=value_error, input_value='email_non_valida', input_type=str]
-birth_date
-  Value error, Data di nascita deve essere nel passato [type=value_error, input_value='3000-01-01', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/value_error
-postal_code
-  Input should be a valid integer, unable to parse string as an integer [type=int_parsing, input_value='ABCDE', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/int_parsing</t>
+          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>{'id': '99ef32ca-eae9-4601-8629-32ae31abf0bd', 'name': 'Lando Regge', 'email': 'email_non_valida', 'birth_date': '3000-01-01', 'phone_number': '+39 3917542572', 'address': 'Piazza Ruberto, 914\n88825, Savelli (KR)', 'city': 'St.Pete', 'postal_code': 'ABCDE', 'state': 'Torino', 'country': 'Montenegro', 'latitude': 42.318689, 'longitude': -156.40589}</t>
+          <t>{"id": "99ef32ca-eae9-4601-8629-32ae31abf0bd", "name": "Lando Regge", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Piazza Ruberto, 914\n88825, Savelli (KR)", "city": "St.Pete", "postal_code": "ABCDE", "state": "Torino", "country": "Montenegro", "latitude": 42.318689, "longitude": -156.40589}</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3 validation errors for Customer
-email
-  value is not a valid email address: An email address must have an @-sign. [type=value_error, input_value='email_non_valida', input_type=str]
-birth_date
-  Value error, Data di nascita deve essere nel passato [type=value_error, input_value='3000-01-01', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/value_error
-postal_code
-  Input should be a valid integer, unable to parse string as an integer [type=int_parsing, input_value='ABCDE', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/int_parsing</t>
+          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>{'id': '402f8b63-5072-44c9-b518-e12f8315636a', 'name': 'Michele Mazzi-Farinelli', 'email': 'email_non_valida', 'birth_date': '3000-01-01', 'phone_number': '+39 3917542572', 'address': 'Strada Olga, 8\n20883, Mezzago (MB)', 'city': 'Le Regine', 'postal_code': 'ABCDE', 'state': 'Cosenza', 'country': 'Olanda', 'latitude': -66.0040975, 'longitude': 128.370492}</t>
+          <t>{"id": "402f8b63-5072-44c9-b518-e12f8315636a", "name": "Michele Mazzi-Farinelli", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Strada Olga, 8\n20883, Mezzago (MB)", "city": "Le Regine", "postal_code": "ABCDE", "state": "Cosenza", "country": "Olanda", "latitude": -66.0040975, "longitude": 128.370492}</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3 validation errors for Customer
-email
-  value is not a valid email address: An email address must have an @-sign. [type=value_error, input_value='email_non_valida', input_type=str]
-birth_date
-  Value error, Data di nascita deve essere nel passato [type=value_error, input_value='3000-01-01', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/value_error
-postal_code
-  Input should be a valid integer, unable to parse string as an integer [type=int_parsing, input_value='ABCDE', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/int_parsing</t>
+          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>{'id': 'a017bf9a-848e-4061-b2c4-cbf89f901147', 'name': 'Dott. Giulia Pezzali', 'email': 'email_non_valida', 'birth_date': '3000-01-01', 'phone_number': '+39 3917542572', 'address': 'Viale Mortati, 33\n13047, San Germano Vercellese (VC)', 'city': 'Inarzo', 'postal_code': 'ABCDE', 'state': 'Pavia', 'country': "Costa d'Avorio", 'latitude': -44.4771955, 'longitude': 125.834881}</t>
+          <t>{"id": "a017bf9a-848e-4061-b2c4-cbf89f901147", "name": "Dott. Giulia Pezzali", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Viale Mortati, 33\n13047, San Germano Vercellese (VC)", "city": "Inarzo", "postal_code": "ABCDE", "state": "Pavia", "country": "Costa d'Avorio", "latitude": -44.4771955, "longitude": 125.834881}</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3 validation errors for Customer
-email
-  value is not a valid email address: An email address must have an @-sign. [type=value_error, input_value='email_non_valida', input_type=str]
-birth_date
-  Value error, Data di nascita deve essere nel passato [type=value_error, input_value='3000-01-01', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/value_error
-postal_code
-  Input should be a valid integer, unable to parse string as an integer [type=int_parsing, input_value='ABCDE', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/int_parsing</t>
+          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>{'id': '532fb55a-3525-4ddc-b368-ec15144c5837', 'name': 'Antonio Chiaramonte', 'email': 'email_non_valida', 'birth_date': '3000-01-01', 'phone_number': '+39 3917542572', 'address': 'Canale Lazzaro, 27 Appartamento 4\n13861, Ailoche (BI)', 'city': 'San Vito Di Altivole', 'postal_code': 'ABCDE', 'state': "L'Aquila", 'country': 'Saint Pierre and Miquelon', 'latitude': 38.8959345, 'longitude': -27.080544}</t>
+          <t>{"id": "532fb55a-3525-4ddc-b368-ec15144c5837", "name": "Antonio Chiaramonte", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Canale Lazzaro, 27 Appartamento 4\n13861, Ailoche (BI)", "city": "San Vito Di Altivole", "postal_code": "ABCDE", "state": "L'Aquila", "country": "Saint Pierre and Miquelon", "latitude": 38.8959345, "longitude": -27.080544}</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3 validation errors for Customer
-email
-  value is not a valid email address: An email address must have an @-sign. [type=value_error, input_value='email_non_valida', input_type=str]
-birth_date
-  Value error, Data di nascita deve essere nel passato [type=value_error, input_value='3000-01-01', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/value_error
-postal_code
-  Input should be a valid integer, unable to parse string as an integer [type=int_parsing, input_value='ABCDE', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/int_parsing</t>
+          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>{'id': '894885a4-9373-4b28-b9e7-ce15236e2ce6', 'name': 'Vincenza Sobrero', 'email': 'email_non_valida', 'birth_date': '3000-01-01', 'phone_number': '+39 3917542572', 'address': "Canale Redi, 75 Appartamento 2\n17038, Villanova D'Albenga (SV)", 'city': 'Ravi', 'postal_code': 'ABCDE', 'state': 'Avellino', 'country': 'Sud Africa', 'latitude': 57.3509865, 'longitude': -137.289091}</t>
+          <t>{"id": "894885a4-9373-4b28-b9e7-ce15236e2ce6", "name": "Vincenza Sobrero", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Canale Redi, 75 Appartamento 2\n17038, Villanova D'Albenga (SV)", "city": "Ravi", "postal_code": "ABCDE", "state": "Avellino", "country": "Sud Africa", "latitude": 57.3509865, "longitude": -137.289091}</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>3 validation errors for Customer
-email
-  value is not a valid email address: An email address must have an @-sign. [type=value_error, input_value='email_non_valida', input_type=str]
-birth_date
-  Value error, Data di nascita deve essere nel passato [type=value_error, input_value='3000-01-01', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/value_error
-postal_code
-  Input should be a valid integer, unable to parse string as an integer [type=int_parsing, input_value='ABCDE', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/int_parsing</t>
+          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>{'id': '1c467026-16de-4d1e-81b7-89412e4aafd7', 'name': 'Emma Vespa', 'email': 'email_non_valida', 'birth_date': '3000-01-01', 'phone_number': '+39 3917542572', 'address': 'Borgo Gioffre, 84\n43030, Marzolara (PR)', 'city': 'Ceppo Morelli', 'postal_code': 'ABCDE', 'state': 'Matera', 'country': 'El Salvador', 'latitude': 77.4680165, 'longitude': -45.453323}</t>
+          <t>{"id": "1c467026-16de-4d1e-81b7-89412e4aafd7", "name": "Emma Vespa", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Borgo Gioffre, 84\n43030, Marzolara (PR)", "city": "Ceppo Morelli", "postal_code": "ABCDE", "state": "Matera", "country": "El Salvador", "latitude": 77.4680165, "longitude": -45.453323}</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3 validation errors for Customer
-email
-  value is not a valid email address: An email address must have an @-sign. [type=value_error, input_value='email_non_valida', input_type=str]
-birth_date
-  Value error, Data di nascita deve essere nel passato [type=value_error, input_value='3000-01-01', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/value_error
-postal_code
-  Input should be a valid integer, unable to parse string as an integer [type=int_parsing, input_value='ABCDE', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/int_parsing</t>
+          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>{'id': 'a2f2736c-6317-4b00-8be9-cd8cceab2e9c', 'name': 'Gianmarco Verdone-Guicciardini', 'email': 'email_non_valida', 'birth_date': '3000-01-01', 'phone_number': '+39 3917542572', 'address': 'Piazza Ignazio, 96 Piano 5\n35026, Conselve (PD)', 'city': 'Drapia', 'postal_code': 'ABCDE', 'state': 'Pordenone', 'country': 'Heard Island and McDonald Islands', 'latitude': -33.660924, 'longitude': -40.092329}</t>
+          <t>{"id": "a2f2736c-6317-4b00-8be9-cd8cceab2e9c", "name": "Gianmarco Verdone-Guicciardini", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Piazza Ignazio, 96 Piano 5\n35026, Conselve (PD)", "city": "Drapia", "postal_code": "ABCDE", "state": "Pordenone", "country": "Heard Island and McDonald Islands", "latitude": -33.660924, "longitude": -40.092329}</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3 validation errors for Customer
-email
-  value is not a valid email address: An email address must have an @-sign. [type=value_error, input_value='email_non_valida', input_type=str]
-birth_date
-  Value error, Data di nascita deve essere nel passato [type=value_error, input_value='3000-01-01', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/value_error
-postal_code
-  Input should be a valid integer, unable to parse string as an integer [type=int_parsing, input_value='ABCDE', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/int_parsing</t>
+          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>{'id': '7d0e3134-f3cb-418a-ae58-abe7cbf04a9c', 'name': 'Elisa Mazzacurati', 'email': 'email_non_valida', 'birth_date': '3000-01-01', 'phone_number': '+39 3917542572', 'address': 'Viale Cavalcanti, 4 Appartamento 8\n65126, Pescara (PE)', 'city': "Sandra'", 'postal_code': 'ABCDE', 'state': 'Massa-Carrara', 'country': 'Qatar', 'latitude': 84.450293, 'longitude': 5.497922}</t>
+          <t>{"id": "7d0e3134-f3cb-418a-ae58-abe7cbf04a9c", "name": "Elisa Mazzacurati", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Viale Cavalcanti, 4 Appartamento 8\n65126, Pescara (PE)", "city": "Sandra'", "postal_code": "ABCDE", "state": "Massa-Carrara", "country": "Qatar", "latitude": 84.450293, "longitude": 5.497922}</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3 validation errors for Customer
-email
-  value is not a valid email address: An email address must have an @-sign. [type=value_error, input_value='email_non_valida', input_type=str]
-birth_date
-  Value error, Data di nascita deve essere nel passato [type=value_error, input_value='3000-01-01', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/value_error
-postal_code
-  Input should be a valid integer, unable to parse string as an integer [type=int_parsing, input_value='ABCDE', input_type=str]
-    For further information visit https://errors.pydantic.dev/2.11/v/int_parsing</t>
+          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Aggiornamento del file .gitignore per includere .env e .docker-compose.yml. Modifiche al README.md per aggiungere nuovi campi opzionali. Ristrutturazione del sistema di salvataggio nel database, passando da SQLite a PostgreSQL. Aggiornamento dei metodi di validazione e report per riflettere i cambiamenti nei dati dei clienti. Rimozione di report obsoleti e miglioramenti nella gestione degli errori.
</commit_message>
<xml_diff>
--- a/output/invalid/customers_invalid.xlsx
+++ b/output/invalid/customers_invalid.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,147 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>data</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>error</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>{"id": "da671afa-1c1c-43b2-870e-b1321e27f076", "name": "Eraldo Gozzano-Valmarana", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Stretto Elvira, 273\n34012, Basovizza (TS)", "city": "San Genesio Atesino", "postal_code": "ABCDE", "state": "Pistoia", "country": "Tajikistan", "latitude": -87.9578655, "longitude": -54.587759}</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>{"id": "a4a2a54f-3833-4d8d-9129-90cad4f58d76", "name": "Rosina Visintini", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Vicolo Magnani, 43\n98141, Giampilieri Marina (ME)", "city": "Caprioli", "postal_code": "ABCDE", "state": "Asti", "country": "Giappone", "latitude": -79.2209, "longitude": -9.437987}</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>{"id": "99ef32ca-eae9-4601-8629-32ae31abf0bd", "name": "Lando Regge", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Piazza Ruberto, 914\n88825, Savelli (KR)", "city": "St.Pete", "postal_code": "ABCDE", "state": "Torino", "country": "Montenegro", "latitude": 42.318689, "longitude": -156.40589}</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>{"id": "402f8b63-5072-44c9-b518-e12f8315636a", "name": "Michele Mazzi-Farinelli", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Strada Olga, 8\n20883, Mezzago (MB)", "city": "Le Regine", "postal_code": "ABCDE", "state": "Cosenza", "country": "Olanda", "latitude": -66.0040975, "longitude": 128.370492}</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>{"id": "a017bf9a-848e-4061-b2c4-cbf89f901147", "name": "Dott. Giulia Pezzali", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Viale Mortati, 33\n13047, San Germano Vercellese (VC)", "city": "Inarzo", "postal_code": "ABCDE", "state": "Pavia", "country": "Costa d'Avorio", "latitude": -44.4771955, "longitude": 125.834881}</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>{"id": "532fb55a-3525-4ddc-b368-ec15144c5837", "name": "Antonio Chiaramonte", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Canale Lazzaro, 27 Appartamento 4\n13861, Ailoche (BI)", "city": "San Vito Di Altivole", "postal_code": "ABCDE", "state": "L'Aquila", "country": "Saint Pierre and Miquelon", "latitude": 38.8959345, "longitude": -27.080544}</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>{"id": "894885a4-9373-4b28-b9e7-ce15236e2ce6", "name": "Vincenza Sobrero", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Canale Redi, 75 Appartamento 2\n17038, Villanova D'Albenga (SV)", "city": "Ravi", "postal_code": "ABCDE", "state": "Avellino", "country": "Sud Africa", "latitude": 57.3509865, "longitude": -137.289091}</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>{"id": "1c467026-16de-4d1e-81b7-89412e4aafd7", "name": "Emma Vespa", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Borgo Gioffre, 84\n43030, Marzolara (PR)", "city": "Ceppo Morelli", "postal_code": "ABCDE", "state": "Matera", "country": "El Salvador", "latitude": 77.4680165, "longitude": -45.453323}</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>{"id": "a2f2736c-6317-4b00-8be9-cd8cceab2e9c", "name": "Gianmarco Verdone-Guicciardini", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Piazza Ignazio, 96 Piano 5\n35026, Conselve (PD)", "city": "Drapia", "postal_code": "ABCDE", "state": "Pordenone", "country": "Heard Island and McDonald Islands", "latitude": -33.660924, "longitude": -40.092329}</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>{"id": "7d0e3134-f3cb-418a-ae58-abe7cbf04a9c", "name": "Elisa Mazzacurati", "email": "email_non_valida", "birth_date": "3000-01-01", "phone_number": "+39 3917542572", "address": "Viale Cavalcanti, 4 Appartamento 8\n65126, Pescara (PE)", "city": "Sandra'", "postal_code": "ABCDE", "state": "Massa-Carrara", "country": "Qatar", "latitude": 84.450293, "longitude": 5.497922}</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>value is not a valid email address: An email address must have an @-sign.; Value error, Data di nascita deve essere nel passato; Input should be a valid integer, unable to parse string as an integer</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>